<commit_message>
Push dates back to 2000-01
Other miscellaneous typos
</commit_message>
<xml_diff>
--- a/data-raw/lito-info.xlsx
+++ b/data-raw/lito-info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GitHub\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>fy_year</t>
   </si>
@@ -82,12 +82,27 @@
   </si>
   <si>
     <t>2016-17</t>
+  </si>
+  <si>
+    <t>2001-02</t>
+  </si>
+  <si>
+    <t>2000-01</t>
+  </si>
+  <si>
+    <t>1999-00</t>
+  </si>
+  <si>
+    <t>1998-99</t>
+  </si>
+  <si>
+    <t>1997-98</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,6 +716,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -736,6 +768,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -888,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,6 +1178,49 @@
         <v>37000</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>150</v>
+      </c>
+      <c r="C17">
+        <v>0.04</v>
+      </c>
+      <c r="D17">
+        <v>20700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>0.04</v>
+      </c>
+      <c r="D18">
+        <v>20700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix derpy LITO entry
</commit_message>
<xml_diff>
--- a/data-raw/lito-info.xlsx
+++ b/data-raw/lito-info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>fy_year</t>
   </si>
@@ -946,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,21 +1231,21 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>445</v>
+        <v>150</v>
       </c>
       <c r="C20">
-        <v>1.4999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D20">
-        <v>37000</v>
+        <v>20700</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>150</v>
@@ -1259,30 +1259,16 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>150</v>
-      </c>
-      <c r="C22">
-        <v>0.04</v>
-      </c>
-      <c r="D22">
-        <v>20700</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>